<commit_message>
dox_project: 1.chapter 5 dynamic table and images  finished start chapter 8
</commit_message>
<xml_diff>
--- a/files/风机基础工程量_test.xlsx
+++ b/files/风机基础工程量_test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
   <workbookPr codeName="ThisWorkbook" hidePivotFieldList="1" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\PycharmProjects\docx_project\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE5D7E67-CA0B-4D75-9543-DF1906DA15BD}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29A565A6-C201-4EE1-AB2E-339F1B707DD0}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5256" yWindow="4824" windowWidth="12360" windowHeight="7848" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="成果输出" sheetId="1" r:id="rId1"/>
@@ -331,9 +331,9 @@
   <numFmts count="5">
     <numFmt numFmtId="176" formatCode="0.00_ "/>
     <numFmt numFmtId="177" formatCode="#&quot;台&quot;"/>
-    <numFmt numFmtId="178" formatCode="#&quot;MW&quot;"/>
     <numFmt numFmtId="179" formatCode="#&quot;kpa&quot;"/>
     <numFmt numFmtId="180" formatCode="#.#&quot;MW&quot;"/>
+    <numFmt numFmtId="182" formatCode="0.00_);[Red]\(0.00\)"/>
   </numFmts>
   <fonts count="13" x14ac:knownFonts="1">
     <font>
@@ -588,7 +588,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -661,9 +661,6 @@
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
@@ -700,9 +697,6 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -726,6 +720,24 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="182" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="182" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="182" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="182" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -733,6 +745,74 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -752,7 +832,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr val="window" lastClr="CCE8CF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -1069,40 +1149,40 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.6" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9" style="3"/>
-    <col min="2" max="2" width="23.75" style="3" customWidth="1"/>
-    <col min="3" max="3" width="17.375" style="3" customWidth="1"/>
-    <col min="4" max="4" width="14.25" style="3" customWidth="1"/>
-    <col min="5" max="5" width="18.25" style="3" customWidth="1"/>
+    <col min="2" max="2" width="23.69921875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="17.3984375" style="3" customWidth="1"/>
+    <col min="4" max="4" width="14.19921875" style="3" customWidth="1"/>
+    <col min="5" max="5" width="18.19921875" style="3" customWidth="1"/>
     <col min="6" max="6" width="10" style="3" bestFit="1" customWidth="1"/>
     <col min="7" max="10" width="9" style="3"/>
-    <col min="11" max="11" width="11.25" style="3" customWidth="1"/>
-    <col min="12" max="12" width="11.625" style="3" customWidth="1"/>
+    <col min="11" max="11" width="11.19921875" style="3" customWidth="1"/>
+    <col min="12" max="12" width="11.59765625" style="3" customWidth="1"/>
     <col min="13" max="13" width="9" style="3"/>
-    <col min="14" max="14" width="11.25" style="3" customWidth="1"/>
+    <col min="14" max="14" width="11.19921875" style="3" customWidth="1"/>
     <col min="15" max="15" width="11.5" style="3" customWidth="1"/>
-    <col min="16" max="16" width="11.75" style="3" customWidth="1"/>
+    <col min="16" max="16" width="11.69921875" style="3" customWidth="1"/>
     <col min="17" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="25" t="s">
+    <row r="1" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="24" t="s">
         <v>59</v>
       </c>
-      <c r="B1" s="45" t="s">
+      <c r="B1" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-    </row>
-    <row r="2" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
+    </row>
+    <row r="2" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>13</v>
       </c>
@@ -1123,7 +1203,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10">
         <v>1</v>
       </c>
@@ -1133,17 +1213,17 @@
       <c r="C3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="32">
+      <c r="D3" s="31">
         <f>风机基础条件输入!D8</f>
         <v>1529.70154599237</v>
       </c>
-      <c r="E3" s="32">
+      <c r="E3" s="31">
         <f>风机基础条件输入!E8</f>
         <v>30594.030919847399</v>
       </c>
       <c r="F3" s="11"/>
     </row>
-    <row r="4" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="10">
         <v>2</v>
       </c>
@@ -1153,17 +1233,17 @@
       <c r="C4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="32">
+      <c r="D4" s="31">
         <f>风机基础条件输入!D9</f>
         <v>0</v>
       </c>
-      <c r="E4" s="32">
+      <c r="E4" s="31">
         <f>风机基础条件输入!E9</f>
         <v>0</v>
       </c>
       <c r="F4" s="11"/>
     </row>
-    <row r="5" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="10">
         <v>3</v>
       </c>
@@ -1173,17 +1253,17 @@
       <c r="C5" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="32" t="e">
+      <c r="D5" s="31">
         <f>风机基础条件输入!D10</f>
-        <v>#N/A</v>
-      </c>
-      <c r="E5" s="32" t="e">
+        <v>990.25667202858529</v>
+      </c>
+      <c r="E5" s="31">
         <f>风机基础条件输入!E10</f>
-        <v>#N/A</v>
+        <v>19805.133440571706</v>
       </c>
       <c r="F5" s="11"/>
     </row>
-    <row r="6" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="10">
         <v>4</v>
       </c>
@@ -1193,17 +1273,17 @@
       <c r="C6" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="32">
+      <c r="D6" s="31">
         <f>风机基础条件输入!D11</f>
         <v>488.96458510865875</v>
       </c>
-      <c r="E6" s="32">
+      <c r="E6" s="31">
         <f>风机基础条件输入!E11</f>
         <v>9779.2917021731755</v>
       </c>
       <c r="F6" s="11"/>
     </row>
-    <row r="7" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="10">
         <v>5</v>
       </c>
@@ -1213,17 +1293,17 @@
       <c r="C7" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="32">
+      <c r="D7" s="31">
         <f>风机基础条件输入!D12</f>
         <v>50.480288855125885</v>
       </c>
-      <c r="E7" s="32">
+      <c r="E7" s="31">
         <f>风机基础条件输入!E12</f>
         <v>1009.6057771025177</v>
       </c>
       <c r="F7" s="11"/>
     </row>
-    <row r="8" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="10">
         <v>6</v>
       </c>
@@ -1233,21 +1313,21 @@
       <c r="C8" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="32">
+      <c r="D8" s="31">
         <f>风机基础条件输入!D13</f>
         <v>48.896458510865877</v>
       </c>
-      <c r="E8" s="32">
+      <c r="E8" s="31">
         <f>风机基础条件输入!E13</f>
         <v>977.92917021731751</v>
       </c>
       <c r="F8" s="11"/>
     </row>
-    <row r="9" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="10">
         <v>7</v>
       </c>
-      <c r="B9" s="27" t="s">
+      <c r="B9" s="26" t="s">
         <v>61</v>
       </c>
       <c r="C9" s="4" t="s">
@@ -1263,14 +1343,14 @@
       </c>
       <c r="F9" s="12"/>
     </row>
-    <row r="10" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="10">
         <v>8</v>
       </c>
-      <c r="B10" s="26" t="s">
+      <c r="B10" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="26" t="s">
+      <c r="C10" s="25" t="s">
         <v>15</v>
       </c>
       <c r="D10" s="5">
@@ -1283,14 +1363,14 @@
       </c>
       <c r="F10" s="12"/>
     </row>
-    <row r="11" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="10">
         <v>9</v>
       </c>
-      <c r="B11" s="27" t="s">
+      <c r="B11" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="C11" s="27" t="s">
+      <c r="C11" s="26" t="s">
         <v>44</v>
       </c>
       <c r="D11" s="5">
@@ -1301,16 +1381,16 @@
         <f>风机基础条件输入!E16</f>
         <v>6400</v>
       </c>
-      <c r="F11" s="42"/>
-    </row>
-    <row r="12" spans="1:6" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="28">
+      <c r="F11" s="40"/>
+    </row>
+    <row r="12" spans="1:6" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="27">
         <v>10</v>
       </c>
-      <c r="B12" s="29" t="s">
+      <c r="B12" s="28" t="s">
         <v>52</v>
       </c>
-      <c r="C12" s="29" t="s">
+      <c r="C12" s="28" t="s">
         <v>53</v>
       </c>
       <c r="D12" s="13">
@@ -1341,81 +1421,81 @@
   <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.5" customWidth="1"/>
-    <col min="2" max="2" width="11.875" customWidth="1"/>
-    <col min="3" max="3" width="13.25" customWidth="1"/>
-    <col min="4" max="5" width="15.375" customWidth="1"/>
+    <col min="2" max="2" width="11.8984375" customWidth="1"/>
+    <col min="3" max="3" width="13.19921875" customWidth="1"/>
+    <col min="4" max="5" width="15.3984375" customWidth="1"/>
     <col min="6" max="6" width="14" customWidth="1"/>
-    <col min="7" max="7" width="13.125" customWidth="1"/>
-    <col min="8" max="9" width="11.875" customWidth="1"/>
+    <col min="7" max="7" width="13.09765625" customWidth="1"/>
+    <col min="8" max="9" width="11.8984375" customWidth="1"/>
     <col min="11" max="11" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.25" customWidth="1"/>
-    <col min="19" max="19" width="10.75" customWidth="1"/>
-    <col min="20" max="20" width="11.25" customWidth="1"/>
+    <col min="13" max="13" width="11.19921875" customWidth="1"/>
+    <col min="19" max="19" width="10.69921875" customWidth="1"/>
+    <col min="20" max="20" width="11.19921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A1" s="38" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="38" t="s">
+      <c r="B1" s="36" t="s">
         <v>55</v>
       </c>
-      <c r="C1" s="39" t="s">
+      <c r="C1" s="37" t="s">
         <v>56</v>
       </c>
-      <c r="D1" s="38" t="s">
+      <c r="D1" s="36" t="s">
         <v>27</v>
       </c>
-      <c r="E1" s="40" t="s">
+      <c r="E1" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="F1" s="31" t="s">
+      <c r="F1" s="30" t="s">
         <v>54</v>
       </c>
-      <c r="G1" s="40" t="s">
+      <c r="G1" s="38" t="s">
         <v>48</v>
       </c>
-      <c r="H1" s="40" t="s">
+      <c r="H1" s="38" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A2" s="33">
-        <v>9</v>
-      </c>
-      <c r="B2" s="34">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="32">
+        <v>7</v>
+      </c>
+      <c r="B2" s="33">
         <v>120</v>
       </c>
-      <c r="C2" s="43">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="D2" s="35">
+      <c r="C2" s="41">
+        <v>2</v>
+      </c>
+      <c r="D2" s="34">
         <v>20</v>
       </c>
-      <c r="E2" s="44" t="s">
+      <c r="E2" s="42" t="s">
         <v>37</v>
       </c>
-      <c r="F2" s="35">
+      <c r="F2" s="44">
         <v>110000</v>
       </c>
-      <c r="G2" s="41">
+      <c r="G2" s="39">
         <v>10</v>
       </c>
-      <c r="H2" s="41">
+      <c r="H2" s="39">
         <f>10-G2</f>
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C3" s="15"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>13</v>
       </c>
@@ -1436,7 +1516,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:8" ht="16.8" x14ac:dyDescent="0.25">
       <c r="A8" s="10">
         <v>1</v>
       </c>
@@ -1446,17 +1526,17 @@
       <c r="C8" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="32">
-        <f t="array" ref="D8">VLOOKUP(E2&amp;F2,IF({1,0},基础数据!$C$21:C36&amp;基础数据!$D$21:$D$36,基础数据!R21:R36),2,0)</f>
+      <c r="D8" s="46">
+        <f t="array" ref="D8">VLOOKUP(E2&amp;F2,IF({1,0},基础数据!$A$21:A36&amp;基础数据!$B$21:$B$36,基础数据!P21:P36),2,0)</f>
         <v>1529.70154599237</v>
       </c>
-      <c r="E8" s="32">
+      <c r="E8" s="46">
         <f>D8*$E$7</f>
         <v>30594.030919847399</v>
       </c>
       <c r="F8" s="11"/>
     </row>
-    <row r="9" spans="1:8" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:8" ht="16.8" x14ac:dyDescent="0.25">
       <c r="A9" s="10">
         <v>2</v>
       </c>
@@ -1466,17 +1546,17 @@
       <c r="C9" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="32">
-        <f t="array" ref="D9">VLOOKUP(E2&amp;F2,IF({1,0},基础数据!$C$21:C36&amp;基础数据!$D$21:$D$36,基础数据!S21:S36),2,0)</f>
+      <c r="D9" s="46">
+        <f t="array" ref="D9">VLOOKUP(E2&amp;F2,IF({1,0},基础数据!$A$21:A36&amp;基础数据!$B$21:$B$36,基础数据!Q21:Q36),2,0)</f>
         <v>0</v>
       </c>
-      <c r="E9" s="32">
+      <c r="E9" s="46">
         <f t="shared" ref="E9:E17" si="0">D9*$E$7</f>
         <v>0</v>
       </c>
       <c r="F9" s="11"/>
     </row>
-    <row r="10" spans="1:8" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:8" ht="16.8" x14ac:dyDescent="0.25">
       <c r="A10" s="10">
         <v>3</v>
       </c>
@@ -1486,17 +1566,17 @@
       <c r="C10" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D10" s="32" t="e">
-        <f>VLOOKUP(E2&amp;F2,IF({1,0},基础数据!$C$21:C36&amp;基础数据!$D$21:$D$36,基础数据!T21:T36),2,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="E10" s="32" t="e">
+      <c r="D10" s="46">
+        <f t="array" ref="D10">VLOOKUP(E2&amp;F2,IF({1,0},基础数据!$A$21:A36&amp;基础数据!$B$21:$B$36,基础数据!R21:R36),2,0)</f>
+        <v>990.25667202858529</v>
+      </c>
+      <c r="E10" s="46">
         <f>D10*$E$7</f>
-        <v>#N/A</v>
+        <v>19805.133440571706</v>
       </c>
       <c r="F10" s="11"/>
     </row>
-    <row r="11" spans="1:8" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:8" ht="16.8" x14ac:dyDescent="0.25">
       <c r="A11" s="10">
         <v>4</v>
       </c>
@@ -1506,17 +1586,17 @@
       <c r="C11" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D11" s="32">
-        <f t="array" ref="D11">VLOOKUP(E2&amp;F2,IF({1,0},基础数据!$C$21:C36&amp;基础数据!$D$21:$D$36,基础数据!P21:P36),2,0)</f>
+      <c r="D11" s="46">
+        <f t="array" ref="D11">VLOOKUP(E2&amp;F2,IF({1,0},基础数据!$A$21:A36&amp;基础数据!$B$21:$B$36,基础数据!N21:N36),2,0)</f>
         <v>488.96458510865875</v>
       </c>
-      <c r="E11" s="32">
+      <c r="E11" s="46">
         <f t="shared" si="0"/>
         <v>9779.2917021731755</v>
       </c>
       <c r="F11" s="11"/>
     </row>
-    <row r="12" spans="1:8" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:8" ht="16.8" x14ac:dyDescent="0.25">
       <c r="A12" s="10">
         <v>5</v>
       </c>
@@ -1526,17 +1606,17 @@
       <c r="C12" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D12" s="32">
-        <f t="array" ref="D12">VLOOKUP(E2&amp;F2,IF({1,0},基础数据!$C$21:C36&amp;基础数据!$D$21:$D$36,基础数据!Q21:Q36),2,0)</f>
+      <c r="D12" s="46">
+        <f t="array" ref="D12">VLOOKUP(E2&amp;F2,IF({1,0},基础数据!$A$21:A36&amp;基础数据!$B$21:$B$36,基础数据!O21:O36),2,0)</f>
         <v>50.480288855125885</v>
       </c>
-      <c r="E12" s="32">
+      <c r="E12" s="46">
         <f t="shared" si="0"/>
         <v>1009.6057771025177</v>
       </c>
       <c r="F12" s="11"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="10">
         <v>6</v>
       </c>
@@ -1546,93 +1626,93 @@
       <c r="C13" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="32">
+      <c r="D13" s="46">
         <f>D11*0.1</f>
         <v>48.896458510865877</v>
       </c>
-      <c r="E13" s="32">
+      <c r="E13" s="46">
         <f t="shared" si="0"/>
         <v>977.92917021731751</v>
       </c>
       <c r="F13" s="11"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="10">
         <v>7</v>
       </c>
-      <c r="B14" s="27" t="s">
+      <c r="B14" s="26" t="s">
         <v>60</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D14" s="5">
+      <c r="D14" s="46">
         <v>1</v>
       </c>
-      <c r="E14" s="5">
+      <c r="E14" s="46">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="F14" s="11"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="10">
         <v>8</v>
       </c>
-      <c r="B15" s="26" t="s">
+      <c r="B15" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="26" t="s">
+      <c r="C15" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="D15" s="5">
-        <v>4</v>
-      </c>
-      <c r="E15" s="5">
+      <c r="D15" s="46">
+        <v>4</v>
+      </c>
+      <c r="E15" s="46">
         <f t="shared" si="0"/>
         <v>80</v>
       </c>
       <c r="F15" s="12"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="10">
         <v>9</v>
       </c>
-      <c r="B16" s="27" t="s">
+      <c r="B16" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="C16" s="27" t="s">
+      <c r="C16" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="D16" s="5">
-        <f t="array" ref="D16">VLOOKUP(E2&amp;F2,IF({1,0},基础数据!$C$21:C36&amp;基础数据!$D$21:$D$36,基础数据!N21:N36),2,0)</f>
+      <c r="D16" s="46">
+        <f t="array" ref="D16">VLOOKUP(E2&amp;F2,IF({1,0},基础数据!$A$21:A36&amp;基础数据!$B$21:$B$36,基础数据!L21:L36),2,0)</f>
         <v>320</v>
       </c>
-      <c r="E16" s="5">
+      <c r="E16" s="46">
         <f t="shared" si="0"/>
         <v>6400</v>
       </c>
       <c r="F16" s="12"/>
     </row>
-    <row r="17" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="28">
+    <row r="17" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="27">
         <v>10</v>
       </c>
-      <c r="B17" s="29" t="s">
+      <c r="B17" s="28" t="s">
         <v>52</v>
       </c>
-      <c r="C17" s="29" t="s">
+      <c r="C17" s="28" t="s">
         <v>53</v>
       </c>
-      <c r="D17" s="37">
-        <f t="array" ref="D17">VLOOKUP(E2&amp;F2,IF({1,0},基础数据!$C$21:C36&amp;基础数据!$D$21:$D$36,基础数据!U21:U36),2,0)</f>
+      <c r="D17" s="47">
+        <f t="array" ref="D17">VLOOKUP(E2&amp;F2,IF({1,0},基础数据!$A$21:A36&amp;基础数据!$B$21:$B$36,基础数据!S21:S36),2,0)</f>
         <v>0</v>
       </c>
-      <c r="E17" s="13">
+      <c r="E17" s="48">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F17" s="30"/>
+      <c r="F17" s="29"/>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
@@ -1684,18 +1764,26 @@
   <dimension ref="A1:V36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21:D32"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="13.25" customWidth="1"/>
-    <col min="4" max="4" width="10.625" customWidth="1"/>
+    <col min="2" max="2" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.19921875" customWidth="1"/>
+    <col min="4" max="4" width="13.69921875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.3984375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.5" customWidth="1"/>
-    <col min="10" max="10" width="11.75" customWidth="1"/>
+    <col min="7" max="7" width="14.3984375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.8984375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.69921875" customWidth="1"/>
+    <col min="13" max="15" width="8.8984375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.3984375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="8.8984375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>20</v>
       </c>
@@ -1720,7 +1808,7 @@
       <c r="K1">
         <v>2</v>
       </c>
-      <c r="M1" s="25" t="s">
+      <c r="M1" s="24" t="s">
         <v>18</v>
       </c>
       <c r="N1" s="20">
@@ -1733,7 +1821,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>20</v>
       </c>
@@ -1758,7 +1846,7 @@
       <c r="K2">
         <v>2.2000000000000002</v>
       </c>
-      <c r="M2" s="25" t="s">
+      <c r="M2" s="24" t="s">
         <v>18</v>
       </c>
       <c r="N2" s="20">
@@ -1771,7 +1859,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -1796,7 +1884,7 @@
       <c r="K3">
         <v>2.5</v>
       </c>
-      <c r="M3" s="25" t="s">
+      <c r="M3" s="24" t="s">
         <v>18</v>
       </c>
       <c r="N3" s="20">
@@ -1809,7 +1897,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -1834,7 +1922,7 @@
       <c r="K4">
         <v>3</v>
       </c>
-      <c r="M4" s="25" t="s">
+      <c r="M4" s="24" t="s">
         <v>18</v>
       </c>
       <c r="N4" s="20">
@@ -1847,7 +1935,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D5" t="s">
         <v>21</v>
       </c>
@@ -1860,7 +1948,7 @@
       <c r="K5">
         <v>3.2</v>
       </c>
-      <c r="M5" s="25" t="s">
+      <c r="M5" s="24" t="s">
         <v>18</v>
       </c>
       <c r="N5" s="20">
@@ -1873,7 +1961,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D6" t="s">
         <v>21</v>
       </c>
@@ -1886,7 +1974,7 @@
       <c r="K6">
         <v>3.3</v>
       </c>
-      <c r="M6" s="25" t="s">
+      <c r="M6" s="24" t="s">
         <v>18</v>
       </c>
       <c r="N6" s="20">
@@ -1899,7 +1987,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D7" t="s">
         <v>21</v>
       </c>
@@ -1912,7 +2000,7 @@
       <c r="K7">
         <v>3.4</v>
       </c>
-      <c r="M7" s="25" t="s">
+      <c r="M7" s="24" t="s">
         <v>18</v>
       </c>
       <c r="N7" s="20">
@@ -1925,14 +2013,14 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D8" t="s">
         <v>21</v>
       </c>
       <c r="E8">
         <v>200</v>
       </c>
-      <c r="M8" s="25" t="s">
+      <c r="M8" s="24" t="s">
         <v>18</v>
       </c>
       <c r="N8" s="20">
@@ -1945,7 +2033,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D9" t="s">
         <v>21</v>
       </c>
@@ -1959,7 +2047,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D10" t="s">
         <v>21</v>
       </c>
@@ -1973,7 +2061,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D11" t="s">
         <v>21</v>
       </c>
@@ -1981,1132 +2069,1132 @@
         <v>260</v>
       </c>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.15">
-      <c r="A19" s="25" t="s">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A19" s="24" t="s">
         <v>64</v>
       </c>
-      <c r="C19" s="25"/>
-    </row>
-    <row r="20" spans="1:22" ht="25.5" x14ac:dyDescent="0.15">
-      <c r="A20" s="25" t="s">
+      <c r="C19" s="24"/>
+    </row>
+    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A20" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="C20" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E20" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="F20" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="G20" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="H20" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="I20" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="J20" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="K20" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="L20" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="M20" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="N20" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="O20" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="P20" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q20" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="R20" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="S20" s="35" t="s">
+        <v>57</v>
+      </c>
+      <c r="T20" s="35" t="s">
+        <v>58</v>
+      </c>
+      <c r="U20" s="24" t="s">
         <v>62</v>
       </c>
-      <c r="B20" s="25" t="s">
+      <c r="V20" s="24" t="s">
         <v>63</v>
       </c>
-      <c r="C20" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="D20" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="E20" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="F20" s="18" t="s">
-        <v>29</v>
-      </c>
-      <c r="G20" s="18" t="s">
-        <v>30</v>
-      </c>
-      <c r="H20" s="19" t="s">
-        <v>31</v>
-      </c>
-      <c r="I20" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="J20" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="K20" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="L20" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="M20" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="N20" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="O20" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="P20" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q20" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="R20" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="S20" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="T20" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="U20" s="36" t="s">
-        <v>57</v>
-      </c>
-      <c r="V20" s="36" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.15">
-      <c r="A21">
-        <v>7</v>
-      </c>
-      <c r="B21">
-        <v>120</v>
-      </c>
-      <c r="C21" s="24" t="s">
+    </row>
+    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A21" s="45" t="s">
         <v>17</v>
       </c>
-      <c r="D21" s="20">
+      <c r="B21" s="45">
         <v>50000</v>
       </c>
-      <c r="E21" s="1">
+      <c r="C21" s="1">
         <v>9.5</v>
       </c>
+      <c r="D21" s="2">
+        <v>4</v>
+      </c>
+      <c r="E21" s="2">
+        <v>4</v>
+      </c>
       <c r="F21" s="2">
-        <v>4</v>
-      </c>
-      <c r="G21" s="2">
-        <v>4</v>
-      </c>
-      <c r="H21" s="2">
         <v>1</v>
       </c>
-      <c r="I21" s="22">
+      <c r="G21" s="22">
         <v>1.2</v>
       </c>
-      <c r="J21" s="22">
+      <c r="H21" s="22">
         <v>1</v>
       </c>
+      <c r="I21" s="22"/>
+      <c r="J21" s="22"/>
       <c r="K21" s="22"/>
       <c r="L21" s="22"/>
-      <c r="M21" s="22"/>
-      <c r="N21" s="22"/>
-      <c r="O21" s="23">
-        <f t="shared" ref="O21:O36" si="0">PI()*E21^2</f>
+      <c r="M21" s="49">
+        <f>PI()*C21^2</f>
         <v>283.5287369864788</v>
       </c>
-      <c r="P21" s="23">
-        <f t="shared" ref="P21:P36" si="1">PI()*E21^2*H21+PI()*G21^2*J21+(E21^2+F21^2+(E21^2*F21^2)^0.5)*I21/3</f>
+      <c r="N21" s="49">
+        <f>PI()*C21^2*F21+PI()*E21^2*H21+(C21^2+D21^2+(C21^2*D21^2)^0.5)*G21/3</f>
         <v>391.49421944391548</v>
       </c>
-      <c r="Q21" s="23">
-        <f t="shared" ref="Q21:Q36" si="2">PI()*(E21+0.1)^2*0.15</f>
+      <c r="O21" s="49">
+        <f>PI()*(C21+0.1)^2*0.15</f>
         <v>43.429376843225299</v>
       </c>
-      <c r="R21" s="23">
-        <f>PI()*(E21+1.3)^2*(H21+I21+J21+0.15)*风机基础条件输入!$G$2/10</f>
+      <c r="P21" s="49">
+        <f>PI()*(C21+1.3)^2*(F21+G21+H21+0.15)*风机基础条件输入!$G$2/10</f>
         <v>1227.5584798342904</v>
       </c>
-      <c r="S21" s="23">
-        <f>PI()*(E21+1.3)^2*(H21+I21+J21+0.15)*风机基础条件输入!$H$2/10</f>
+      <c r="Q21" s="49">
+        <f>PI()*(C21+1.3)^2*(F21+G21+H21+0.15)*风机基础条件输入!$H$2/10</f>
         <v>0</v>
       </c>
-      <c r="T21" s="23">
-        <f t="shared" ref="T21:T36" si="3">R21+S21-P21-Q21</f>
+      <c r="R21" s="49">
+        <f t="shared" ref="R21:R36" si="0">P21+Q21-N21-O21</f>
         <v>792.63488354714968</v>
       </c>
-      <c r="U21" s="23"/>
-    </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.15">
-      <c r="A22">
+      <c r="S21" s="23"/>
+      <c r="U21">
         <v>7</v>
       </c>
-      <c r="B22">
+      <c r="V21">
         <v>120</v>
       </c>
-      <c r="C22" s="24" t="s">
+    </row>
+    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A22" s="45" t="s">
         <v>17</v>
       </c>
-      <c r="D22" s="20">
+      <c r="B22" s="45">
         <v>60000</v>
       </c>
-      <c r="E22" s="1">
+      <c r="C22" s="1">
         <v>10</v>
       </c>
+      <c r="D22" s="2">
+        <v>4</v>
+      </c>
+      <c r="E22" s="2">
+        <v>4</v>
+      </c>
       <c r="F22" s="2">
-        <v>4</v>
-      </c>
-      <c r="G22" s="2">
-        <v>4</v>
-      </c>
-      <c r="H22" s="2">
         <v>1</v>
       </c>
-      <c r="I22" s="22">
+      <c r="G22" s="22">
         <v>1.4</v>
       </c>
-      <c r="J22" s="22">
+      <c r="H22" s="22">
         <v>1</v>
       </c>
+      <c r="I22" s="22"/>
+      <c r="J22" s="22"/>
       <c r="K22" s="22"/>
       <c r="L22" s="22"/>
-      <c r="M22" s="22"/>
-      <c r="N22" s="22"/>
-      <c r="O22" s="23">
+      <c r="M22" s="49">
+        <f t="shared" ref="M22:M36" si="1">PI()*C22^2</f>
+        <v>314.15926535897933</v>
+      </c>
+      <c r="N22" s="49">
+        <f t="shared" ref="N21:N36" si="2">PI()*C22^2*F22+PI()*E22^2*H22+(C22^2+D22^2+(C22^2*D22^2)^0.5)*G22/3</f>
+        <v>437.22474781641603</v>
+      </c>
+      <c r="O22" s="49">
+        <f t="shared" ref="O21:O36" si="3">PI()*(C22+0.1)^2*0.15</f>
+        <v>48.071079988904216</v>
+      </c>
+      <c r="P22" s="49">
+        <f>PI()*(C22+1.3)^2*(F22+G22+H22+0.15)*风机基础条件输入!$G$2/10</f>
+        <v>1424.0823790759266</v>
+      </c>
+      <c r="Q22" s="49">
+        <f>PI()*(C22+1.3)^2*(F22+G22+H22+0.15)*风机基础条件输入!$H$2/10</f>
+        <v>0</v>
+      </c>
+      <c r="R22" s="49">
         <f t="shared" si="0"/>
-        <v>314.15926535897933</v>
-      </c>
-      <c r="P22" s="23">
-        <f t="shared" si="1"/>
-        <v>437.22474781641603</v>
-      </c>
-      <c r="Q22" s="23">
-        <f t="shared" si="2"/>
-        <v>48.071079988904216</v>
-      </c>
-      <c r="R22" s="23">
-        <f>PI()*(E22+1.3)^2*(H22+I22+J22+0.15)*风机基础条件输入!$G$2/10</f>
-        <v>1424.0823790759266</v>
-      </c>
-      <c r="S22" s="23">
-        <f>PI()*(E22+1.3)^2*(H22+I22+J22+0.15)*风机基础条件输入!$H$2/10</f>
-        <v>0</v>
-      </c>
-      <c r="T22" s="23">
-        <f t="shared" si="3"/>
         <v>938.78655127060631</v>
       </c>
-      <c r="U22" s="23"/>
-    </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.15">
-      <c r="A23">
+      <c r="S22" s="23"/>
+      <c r="U22">
         <v>7</v>
       </c>
-      <c r="B23">
+      <c r="V22">
         <v>120</v>
       </c>
-      <c r="C23" s="24" t="s">
+    </row>
+    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A23" s="45" t="s">
         <v>17</v>
       </c>
-      <c r="D23" s="20">
+      <c r="B23" s="45">
         <v>70000</v>
       </c>
-      <c r="E23" s="1">
+      <c r="C23" s="1">
         <v>10.25</v>
       </c>
+      <c r="D23" s="2">
+        <v>4</v>
+      </c>
+      <c r="E23" s="2">
+        <v>4</v>
+      </c>
       <c r="F23" s="2">
-        <v>4</v>
-      </c>
-      <c r="G23" s="2">
-        <v>4</v>
-      </c>
-      <c r="H23" s="2">
         <v>1.2</v>
       </c>
-      <c r="I23" s="22">
+      <c r="G23" s="22">
         <v>1.4</v>
       </c>
-      <c r="J23" s="22">
+      <c r="H23" s="22">
         <v>1</v>
       </c>
+      <c r="I23" s="22"/>
+      <c r="J23" s="22"/>
       <c r="K23" s="22"/>
       <c r="L23" s="22"/>
-      <c r="M23" s="22"/>
-      <c r="N23" s="22"/>
-      <c r="O23" s="23">
+      <c r="M23" s="49">
+        <f t="shared" si="1"/>
+        <v>330.06357816777762</v>
+      </c>
+      <c r="N23" s="49">
+        <f t="shared" si="2"/>
+        <v>521.97094292543647</v>
+      </c>
+      <c r="O23" s="49">
+        <f t="shared" si="3"/>
+        <v>50.480288855125885</v>
+      </c>
+      <c r="P23" s="49">
+        <f>PI()*(C23+1.3)^2*(F23+G23+H23+0.15)*风机基础条件输入!$G$2/10</f>
+        <v>1571.6111773894213</v>
+      </c>
+      <c r="Q23" s="49">
+        <f>PI()*(C23+1.3)^2*(F23+G23+H23+0.15)*风机基础条件输入!$H$2/10</f>
+        <v>0</v>
+      </c>
+      <c r="R23" s="49">
         <f t="shared" si="0"/>
-        <v>330.06357816777762</v>
-      </c>
-      <c r="P23" s="23">
-        <f t="shared" si="1"/>
-        <v>521.97094292543647</v>
-      </c>
-      <c r="Q23" s="23">
-        <f t="shared" si="2"/>
-        <v>50.480288855125885</v>
-      </c>
-      <c r="R23" s="23">
-        <f>PI()*(E23+1.3)^2*(H23+I23+J23+0.15)*风机基础条件输入!$G$2/10</f>
-        <v>1571.6111773894213</v>
-      </c>
-      <c r="S23" s="23">
-        <f>PI()*(E23+1.3)^2*(H23+I23+J23+0.15)*风机基础条件输入!$H$2/10</f>
-        <v>0</v>
-      </c>
-      <c r="T23" s="23">
-        <f t="shared" si="3"/>
         <v>999.15994560885895</v>
       </c>
-      <c r="U23" s="23"/>
-    </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.15">
-      <c r="A24">
+      <c r="S23" s="23"/>
+      <c r="U23">
         <v>7</v>
       </c>
-      <c r="B24">
+      <c r="V23">
         <v>120</v>
       </c>
-      <c r="C24" s="24" t="s">
+    </row>
+    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A24" s="45" t="s">
         <v>17</v>
       </c>
-      <c r="D24" s="20">
+      <c r="B24" s="45">
         <v>80000</v>
       </c>
+      <c r="C24" s="2">
+        <v>10.5</v>
+      </c>
+      <c r="D24" s="2">
+        <v>4</v>
+      </c>
       <c r="E24" s="2">
-        <v>10.5</v>
+        <v>4</v>
       </c>
       <c r="F24" s="2">
-        <v>4</v>
-      </c>
-      <c r="G24" s="2">
-        <v>4</v>
-      </c>
-      <c r="H24" s="2">
         <v>1.2</v>
       </c>
-      <c r="I24" s="22">
+      <c r="G24" s="22">
         <v>1.4</v>
       </c>
-      <c r="J24" s="22">
+      <c r="H24" s="22">
         <v>1</v>
       </c>
+      <c r="I24" s="22"/>
+      <c r="J24" s="22"/>
       <c r="K24" s="22"/>
       <c r="L24" s="22"/>
-      <c r="M24" s="22"/>
-      <c r="N24" s="22"/>
-      <c r="O24" s="23">
+      <c r="M24" s="49">
+        <f t="shared" si="1"/>
+        <v>346.36059005827468</v>
+      </c>
+      <c r="N24" s="49">
+        <f t="shared" si="2"/>
+        <v>544.41485719403295</v>
+      </c>
+      <c r="O24" s="49">
+        <f t="shared" si="3"/>
+        <v>52.948402583602373</v>
+      </c>
+      <c r="P24" s="49">
+        <f>PI()*(C24+1.3)^2*(F24+G24+H24+0.15)*风机基础条件输入!$G$2/10</f>
+        <v>1640.3826040719105</v>
+      </c>
+      <c r="Q24" s="49">
+        <f>PI()*(C24+1.3)^2*(F24+G24+H24+0.15)*风机基础条件输入!$H$2/10</f>
+        <v>0</v>
+      </c>
+      <c r="R24" s="49">
         <f t="shared" si="0"/>
-        <v>346.36059005827468</v>
-      </c>
-      <c r="P24" s="23">
-        <f t="shared" si="1"/>
-        <v>544.41485719403295</v>
-      </c>
-      <c r="Q24" s="23">
-        <f t="shared" si="2"/>
-        <v>52.948402583602373</v>
-      </c>
-      <c r="R24" s="23">
-        <f>PI()*(E24+1.3)^2*(H24+I24+J24+0.15)*风机基础条件输入!$G$2/10</f>
-        <v>1640.3826040719105</v>
-      </c>
-      <c r="S24" s="23">
-        <f>PI()*(E24+1.3)^2*(H24+I24+J24+0.15)*风机基础条件输入!$H$2/10</f>
-        <v>0</v>
-      </c>
-      <c r="T24" s="23">
-        <f t="shared" si="3"/>
         <v>1043.0193442942752</v>
       </c>
-      <c r="U24" s="23"/>
-    </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.15">
-      <c r="A25">
+      <c r="S24" s="23"/>
+      <c r="U24">
         <v>7</v>
       </c>
-      <c r="B25">
+      <c r="V24">
         <v>120</v>
       </c>
-      <c r="C25" s="24" t="s">
+    </row>
+    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A25" s="45" t="s">
         <v>17</v>
       </c>
-      <c r="D25" s="20">
+      <c r="B25" s="45">
         <v>90000</v>
       </c>
+      <c r="C25" s="2">
+        <v>10.75</v>
+      </c>
+      <c r="D25" s="2">
+        <v>4</v>
+      </c>
       <c r="E25" s="2">
-        <v>10.75</v>
+        <v>4</v>
       </c>
       <c r="F25" s="2">
-        <v>4</v>
-      </c>
-      <c r="G25" s="2">
-        <v>4</v>
-      </c>
-      <c r="H25" s="2">
         <v>1.2</v>
       </c>
-      <c r="I25" s="22">
+      <c r="G25" s="22">
         <v>1.5</v>
       </c>
-      <c r="J25" s="22">
+      <c r="H25" s="22">
         <v>1</v>
       </c>
+      <c r="I25" s="22"/>
+      <c r="J25" s="22"/>
       <c r="K25" s="22"/>
       <c r="L25" s="22"/>
-      <c r="M25" s="22"/>
-      <c r="N25" s="22"/>
-      <c r="O25" s="23">
+      <c r="M25" s="49">
+        <f t="shared" si="1"/>
+        <v>363.05030103047045</v>
+      </c>
+      <c r="N25" s="49">
+        <f t="shared" si="2"/>
+        <v>573.20709369400129</v>
+      </c>
+      <c r="O25" s="49">
+        <f t="shared" si="3"/>
+        <v>55.475421174333661</v>
+      </c>
+      <c r="P25" s="49">
+        <f>PI()*(C25+1.3)^2*(F25+G25+H25+0.15)*风机基础条件输入!$G$2/10</f>
+        <v>1756.2433630390574</v>
+      </c>
+      <c r="Q25" s="49">
+        <f>PI()*(C25+1.3)^2*(F25+G25+H25+0.15)*风机基础条件输入!$H$2/10</f>
+        <v>0</v>
+      </c>
+      <c r="R25" s="49">
         <f t="shared" si="0"/>
-        <v>363.05030103047045</v>
-      </c>
-      <c r="P25" s="23">
-        <f t="shared" si="1"/>
-        <v>573.20709369400129</v>
-      </c>
-      <c r="Q25" s="23">
-        <f t="shared" si="2"/>
-        <v>55.475421174333661</v>
-      </c>
-      <c r="R25" s="23">
-        <f>PI()*(E25+1.3)^2*(H25+I25+J25+0.15)*风机基础条件输入!$G$2/10</f>
-        <v>1756.2433630390574</v>
-      </c>
-      <c r="S25" s="23">
-        <f>PI()*(E25+1.3)^2*(H25+I25+J25+0.15)*风机基础条件输入!$H$2/10</f>
-        <v>0</v>
-      </c>
-      <c r="T25" s="23">
-        <f t="shared" si="3"/>
         <v>1127.5608481707225</v>
       </c>
-      <c r="U25" s="23"/>
-    </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.15">
-      <c r="A26">
+      <c r="S25" s="23"/>
+      <c r="U25">
         <v>7</v>
       </c>
-      <c r="B26">
+      <c r="V25">
         <v>120</v>
       </c>
-      <c r="C26" s="24" t="s">
+    </row>
+    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A26" s="45" t="s">
         <v>17</v>
       </c>
-      <c r="D26" s="20">
+      <c r="B26" s="45">
         <v>100000</v>
       </c>
-      <c r="E26" s="1">
+      <c r="C26" s="1">
         <v>11</v>
       </c>
+      <c r="D26" s="2">
+        <v>4</v>
+      </c>
+      <c r="E26" s="2">
+        <v>4</v>
+      </c>
       <c r="F26" s="2">
-        <v>4</v>
-      </c>
-      <c r="G26" s="2">
-        <v>4</v>
-      </c>
-      <c r="H26" s="2">
         <v>1.2</v>
       </c>
-      <c r="I26" s="22">
+      <c r="G26" s="22">
         <v>1.6</v>
       </c>
-      <c r="J26" s="22">
+      <c r="H26" s="22">
         <v>1</v>
       </c>
+      <c r="I26" s="22"/>
+      <c r="J26" s="22"/>
       <c r="K26" s="22"/>
       <c r="L26" s="22"/>
-      <c r="M26" s="22"/>
-      <c r="N26" s="22"/>
-      <c r="O26" s="23">
+      <c r="M26" s="49">
+        <f t="shared" si="1"/>
+        <v>380.13271108436498</v>
+      </c>
+      <c r="N26" s="49">
+        <f t="shared" si="2"/>
+        <v>602.95806909200803</v>
+      </c>
+      <c r="O26" s="49">
+        <f t="shared" si="3"/>
+        <v>58.061344627319755</v>
+      </c>
+      <c r="P26" s="49">
+        <f>PI()*(C26+1.3)^2*(F26+G26+H26+0.15)*风机基础条件输入!$G$2/10</f>
+        <v>1877.4016326183196</v>
+      </c>
+      <c r="Q26" s="49">
+        <f>PI()*(C26+1.3)^2*(F26+G26+H26+0.15)*风机基础条件输入!$H$2/10</f>
+        <v>0</v>
+      </c>
+      <c r="R26" s="49">
         <f t="shared" si="0"/>
-        <v>380.13271108436498</v>
-      </c>
-      <c r="P26" s="23">
-        <f t="shared" si="1"/>
-        <v>602.95806909200803</v>
-      </c>
-      <c r="Q26" s="23">
-        <f t="shared" si="2"/>
-        <v>58.061344627319755</v>
-      </c>
-      <c r="R26" s="23">
-        <f>PI()*(E26+1.3)^2*(H26+I26+J26+0.15)*风机基础条件输入!$G$2/10</f>
-        <v>1877.4016326183196</v>
-      </c>
-      <c r="S26" s="23">
-        <f>PI()*(E26+1.3)^2*(H26+I26+J26+0.15)*风机基础条件输入!$H$2/10</f>
-        <v>0</v>
-      </c>
-      <c r="T26" s="23">
-        <f t="shared" si="3"/>
         <v>1216.3822188989918</v>
       </c>
-      <c r="U26" s="23"/>
-    </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.15">
-      <c r="A27">
+      <c r="S26" s="23"/>
+      <c r="U26">
         <v>7</v>
       </c>
-      <c r="B27">
+      <c r="V26">
         <v>120</v>
       </c>
-      <c r="C27" s="24" t="s">
+    </row>
+    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A27" s="45" t="s">
         <v>17</v>
       </c>
-      <c r="D27" s="20">
+      <c r="B27" s="45">
         <v>110000</v>
       </c>
-      <c r="E27" s="1">
+      <c r="C27" s="1">
         <v>11.5</v>
       </c>
+      <c r="D27" s="2">
+        <v>4</v>
+      </c>
+      <c r="E27" s="2">
+        <v>4</v>
+      </c>
       <c r="F27" s="2">
-        <v>4</v>
-      </c>
-      <c r="G27" s="2">
-        <v>4</v>
-      </c>
-      <c r="H27" s="2">
         <v>1.3</v>
       </c>
-      <c r="I27" s="22">
+      <c r="G27" s="22">
         <v>1.6</v>
       </c>
-      <c r="J27" s="22">
+      <c r="H27" s="22">
         <v>1</v>
       </c>
+      <c r="I27" s="22"/>
+      <c r="J27" s="22"/>
       <c r="K27" s="22"/>
       <c r="L27" s="22"/>
-      <c r="M27" s="22"/>
-      <c r="N27" s="22"/>
-      <c r="O27" s="23">
+      <c r="M27" s="49">
+        <f t="shared" si="1"/>
+        <v>415.47562843725012</v>
+      </c>
+      <c r="N27" s="49">
+        <f t="shared" si="2"/>
+        <v>693.983799425862</v>
+      </c>
+      <c r="O27" s="49">
+        <f t="shared" si="3"/>
+        <v>63.409906120056384</v>
+      </c>
+      <c r="P27" s="49">
+        <f>PI()*(C27+1.3)^2*(F27+G27+H27+0.15)*风机基础条件输入!$G$2/10</f>
+        <v>2084.6100884748148</v>
+      </c>
+      <c r="Q27" s="49">
+        <f>PI()*(C27+1.3)^2*(F27+G27+H27+0.15)*风机基础条件输入!$H$2/10</f>
+        <v>0</v>
+      </c>
+      <c r="R27" s="49">
         <f t="shared" si="0"/>
-        <v>415.47562843725012</v>
-      </c>
-      <c r="P27" s="23">
-        <f t="shared" si="1"/>
-        <v>693.983799425862</v>
-      </c>
-      <c r="Q27" s="23">
-        <f t="shared" si="2"/>
-        <v>63.409906120056384</v>
-      </c>
-      <c r="R27" s="23">
-        <f>PI()*(E27+1.3)^2*(H27+I27+J27+0.15)*风机基础条件输入!$G$2/10</f>
-        <v>2084.6100884748148</v>
-      </c>
-      <c r="S27" s="23">
-        <f>PI()*(E27+1.3)^2*(H27+I27+J27+0.15)*风机基础条件输入!$H$2/10</f>
-        <v>0</v>
-      </c>
-      <c r="T27" s="23">
-        <f t="shared" si="3"/>
         <v>1327.2163829288966</v>
       </c>
-      <c r="U27" s="23"/>
-    </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.15">
-      <c r="A28">
+      <c r="S27" s="23"/>
+      <c r="U27">
         <v>7</v>
       </c>
-      <c r="B28">
+      <c r="V27">
         <v>120</v>
       </c>
-      <c r="C28" s="24" t="s">
+    </row>
+    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A28" s="45" t="s">
         <v>17</v>
       </c>
-      <c r="D28" s="20">
+      <c r="B28" s="45">
         <v>120000</v>
       </c>
-      <c r="E28" s="21">
+      <c r="C28" s="21">
         <v>12</v>
       </c>
+      <c r="D28" s="2">
+        <v>4</v>
+      </c>
+      <c r="E28" s="2">
+        <v>4</v>
+      </c>
       <c r="F28" s="2">
-        <v>4</v>
-      </c>
-      <c r="G28" s="2">
-        <v>4</v>
-      </c>
-      <c r="H28" s="2">
         <v>1.4</v>
       </c>
-      <c r="I28" s="22">
+      <c r="G28" s="22">
         <v>1.6</v>
       </c>
-      <c r="J28" s="22">
+      <c r="H28" s="22">
         <v>1</v>
       </c>
+      <c r="I28" s="22"/>
+      <c r="J28" s="22"/>
       <c r="K28" s="22"/>
       <c r="L28" s="22"/>
-      <c r="M28" s="22"/>
-      <c r="N28" s="22"/>
-      <c r="O28" s="23">
+      <c r="M28" s="49">
+        <f t="shared" si="1"/>
+        <v>452.38934211693021</v>
+      </c>
+      <c r="N28" s="49">
+        <f t="shared" si="2"/>
+        <v>794.54389475447238</v>
+      </c>
+      <c r="O28" s="49">
+        <f t="shared" si="3"/>
+        <v>68.994087061812237</v>
+      </c>
+      <c r="P28" s="49">
+        <f>PI()*(C28+1.3)^2*(F28+G28+H28+0.15)*风机基础条件输入!$G$2/10</f>
+        <v>2306.222746648019</v>
+      </c>
+      <c r="Q28" s="49">
+        <f>PI()*(C28+1.3)^2*(F28+G28+H28+0.15)*风机基础条件输入!$H$2/10</f>
+        <v>0</v>
+      </c>
+      <c r="R28" s="49">
         <f t="shared" si="0"/>
-        <v>452.38934211693021</v>
-      </c>
-      <c r="P28" s="23">
+        <v>1442.6847648317344</v>
+      </c>
+      <c r="S28" s="23"/>
+      <c r="U28">
+        <v>7</v>
+      </c>
+      <c r="V28">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A29" s="45" t="s">
+        <v>37</v>
+      </c>
+      <c r="B29" s="45">
+        <v>50000</v>
+      </c>
+      <c r="C29" s="1">
+        <v>9</v>
+      </c>
+      <c r="D29" s="2">
+        <v>4</v>
+      </c>
+      <c r="E29" s="2">
+        <v>4</v>
+      </c>
+      <c r="F29" s="2">
+        <v>1</v>
+      </c>
+      <c r="G29" s="22">
+        <v>1</v>
+      </c>
+      <c r="H29" s="22">
+        <v>1</v>
+      </c>
+      <c r="I29" s="22">
+        <v>0.6</v>
+      </c>
+      <c r="J29" s="22">
+        <v>20</v>
+      </c>
+      <c r="K29" s="22">
+        <v>10</v>
+      </c>
+      <c r="L29" s="22">
+        <f t="shared" ref="L29:L36" si="4">J29*K29</f>
+        <v>200</v>
+      </c>
+      <c r="M29" s="49">
         <f t="shared" si="1"/>
-        <v>794.54389475447238</v>
-      </c>
-      <c r="Q28" s="23">
+        <v>254.46900494077323</v>
+      </c>
+      <c r="N29" s="49">
         <f t="shared" si="2"/>
-        <v>68.994087061812237</v>
-      </c>
-      <c r="R28" s="23">
-        <f>PI()*(E28+1.3)^2*(H28+I28+J28+0.15)*风机基础条件输入!$G$2/10</f>
-        <v>2306.222746648019</v>
-      </c>
-      <c r="S28" s="23">
-        <f>PI()*(E28+1.3)^2*(H28+I28+J28+0.15)*风机基础条件输入!$H$2/10</f>
+        <v>349.06782073154324</v>
+      </c>
+      <c r="O29" s="49">
+        <f t="shared" si="3"/>
+        <v>39.023293146565614</v>
+      </c>
+      <c r="P29" s="49">
+        <f>PI()*(C29+1.3)^2*(F29+G29+H29+0.15)*风机基础条件输入!$G$2/10</f>
+        <v>1049.8684285509248</v>
+      </c>
+      <c r="Q29" s="49">
+        <f>PI()*(C29+1.3)^2*(F29+G29+H29+0.15)*风机基础条件输入!$H$2/10</f>
         <v>0</v>
       </c>
-      <c r="T28" s="23">
-        <f t="shared" si="3"/>
-        <v>1442.6847648317344</v>
-      </c>
-      <c r="U28" s="23"/>
-    </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.15">
-      <c r="A29">
+      <c r="R29" s="49">
+        <f t="shared" si="0"/>
+        <v>661.77731467281603</v>
+      </c>
+      <c r="S29" s="23"/>
+      <c r="U29">
         <v>7</v>
       </c>
-      <c r="B29">
+      <c r="V29">
         <v>120</v>
       </c>
-      <c r="C29" s="24" t="s">
+    </row>
+    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A30" s="45" t="s">
         <v>37</v>
       </c>
-      <c r="D29" s="20">
-        <v>50000</v>
-      </c>
-      <c r="E29" s="1">
-        <v>9</v>
-      </c>
-      <c r="F29" s="2">
-        <v>4</v>
-      </c>
-      <c r="G29" s="2">
-        <v>4</v>
-      </c>
-      <c r="H29" s="2">
+      <c r="B30" s="45">
+        <v>60000</v>
+      </c>
+      <c r="C30" s="1">
+        <v>9.5</v>
+      </c>
+      <c r="D30" s="2">
+        <v>4</v>
+      </c>
+      <c r="E30" s="2">
+        <v>4</v>
+      </c>
+      <c r="F30" s="2">
         <v>1</v>
       </c>
-      <c r="I29" s="22">
+      <c r="G30" s="22">
+        <v>1.2</v>
+      </c>
+      <c r="H30" s="22">
         <v>1</v>
       </c>
-      <c r="J29" s="22">
-        <v>1</v>
-      </c>
-      <c r="K29" s="22">
+      <c r="I30" s="22">
         <v>0.6</v>
       </c>
-      <c r="L29" s="22">
-        <v>20</v>
-      </c>
-      <c r="M29" s="22">
+      <c r="J30" s="22">
+        <v>22</v>
+      </c>
+      <c r="K30" s="22">
         <v>10</v>
       </c>
-      <c r="N29" s="22">
-        <f t="shared" ref="N29:N36" si="4">L29*M29</f>
-        <v>200</v>
-      </c>
-      <c r="O29" s="23">
-        <f t="shared" si="0"/>
-        <v>254.46900494077323</v>
-      </c>
-      <c r="P29" s="23">
-        <f t="shared" si="1"/>
-        <v>349.06782073154324</v>
-      </c>
-      <c r="Q29" s="23">
-        <f t="shared" si="2"/>
-        <v>39.023293146565614</v>
-      </c>
-      <c r="R29" s="23">
-        <f>PI()*(E29+1.3)^2*(H29+I29+J29+0.15)*风机基础条件输入!$G$2/10</f>
-        <v>1049.8684285509248</v>
-      </c>
-      <c r="S29" s="23">
-        <f>PI()*(E29+1.3)^2*(H29+I29+J29+0.15)*风机基础条件输入!$H$2/10</f>
-        <v>0</v>
-      </c>
-      <c r="T29" s="23">
-        <f t="shared" si="3"/>
-        <v>661.77731467281603</v>
-      </c>
-      <c r="U29" s="23"/>
-    </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.15">
-      <c r="A30">
-        <v>7</v>
-      </c>
-      <c r="B30">
-        <v>120</v>
-      </c>
-      <c r="C30" s="24" t="s">
-        <v>37</v>
-      </c>
-      <c r="D30" s="20">
-        <v>60000</v>
-      </c>
-      <c r="E30" s="1">
-        <v>9.5</v>
-      </c>
-      <c r="F30" s="2">
-        <v>4</v>
-      </c>
-      <c r="G30" s="2">
-        <v>4</v>
-      </c>
-      <c r="H30" s="2">
-        <v>1</v>
-      </c>
-      <c r="I30" s="22">
-        <v>1.2</v>
-      </c>
-      <c r="J30" s="22">
-        <v>1</v>
-      </c>
-      <c r="K30" s="22">
-        <v>0.6</v>
-      </c>
       <c r="L30" s="22">
-        <v>22</v>
-      </c>
-      <c r="M30" s="22">
-        <v>10</v>
-      </c>
-      <c r="N30" s="22">
         <f t="shared" si="4"/>
         <v>220</v>
       </c>
-      <c r="O30" s="23">
+      <c r="M30" s="49">
+        <f t="shared" si="1"/>
+        <v>283.5287369864788</v>
+      </c>
+      <c r="N30" s="49">
+        <f t="shared" si="2"/>
+        <v>391.49421944391548</v>
+      </c>
+      <c r="O30" s="49">
+        <f t="shared" si="3"/>
+        <v>43.429376843225299</v>
+      </c>
+      <c r="P30" s="49">
+        <f>PI()*(C30+1.3)^2*(F30+G30+H30+0.15)*风机基础条件输入!$G$2/10</f>
+        <v>1227.5584798342904</v>
+      </c>
+      <c r="Q30" s="49">
+        <f>PI()*(C30+1.3)^2*(F30+G30+H30+0.15)*风机基础条件输入!$H$2/10</f>
+        <v>0</v>
+      </c>
+      <c r="R30" s="49">
         <f t="shared" si="0"/>
-        <v>283.5287369864788</v>
-      </c>
-      <c r="P30" s="23">
-        <f t="shared" si="1"/>
-        <v>391.49421944391548</v>
-      </c>
-      <c r="Q30" s="23">
-        <f t="shared" si="2"/>
-        <v>43.429376843225299</v>
-      </c>
-      <c r="R30" s="23">
-        <f>PI()*(E30+1.3)^2*(H30+I30+J30+0.15)*风机基础条件输入!$G$2/10</f>
-        <v>1227.5584798342904</v>
-      </c>
-      <c r="S30" s="23">
-        <f>PI()*(E30+1.3)^2*(H30+I30+J30+0.15)*风机基础条件输入!$H$2/10</f>
-        <v>0</v>
-      </c>
-      <c r="T30" s="23">
-        <f t="shared" si="3"/>
         <v>792.63488354714968</v>
       </c>
-      <c r="U30" s="23"/>
-    </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.15">
-      <c r="A31">
+      <c r="S30" s="23"/>
+      <c r="U30">
         <v>7</v>
       </c>
-      <c r="B31">
+      <c r="V30">
         <v>120</v>
       </c>
-      <c r="C31" s="24" t="s">
+    </row>
+    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A31" s="45" t="s">
         <v>37</v>
       </c>
-      <c r="D31" s="20">
+      <c r="B31" s="45">
         <v>70000</v>
       </c>
-      <c r="E31" s="1">
+      <c r="C31" s="1">
         <v>9.5</v>
       </c>
+      <c r="D31" s="2">
+        <v>4</v>
+      </c>
+      <c r="E31" s="2">
+        <v>4</v>
+      </c>
       <c r="F31" s="2">
-        <v>4</v>
-      </c>
-      <c r="G31" s="2">
-        <v>4</v>
-      </c>
-      <c r="H31" s="2">
         <v>1</v>
       </c>
+      <c r="G31" s="22">
+        <v>1.2</v>
+      </c>
+      <c r="H31" s="22">
+        <v>1</v>
+      </c>
       <c r="I31" s="22">
-        <v>1.2</v>
+        <v>0.6</v>
       </c>
       <c r="J31" s="22">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="K31" s="22">
-        <v>0.6</v>
+        <v>10</v>
       </c>
       <c r="L31" s="22">
-        <v>24</v>
-      </c>
-      <c r="M31" s="22">
-        <v>10</v>
-      </c>
-      <c r="N31" s="22">
         <f t="shared" si="4"/>
         <v>240</v>
       </c>
-      <c r="O31" s="23">
+      <c r="M31" s="49">
+        <f t="shared" si="1"/>
+        <v>283.5287369864788</v>
+      </c>
+      <c r="N31" s="49">
+        <f t="shared" si="2"/>
+        <v>391.49421944391548</v>
+      </c>
+      <c r="O31" s="49">
+        <f t="shared" si="3"/>
+        <v>43.429376843225299</v>
+      </c>
+      <c r="P31" s="49">
+        <f>PI()*(C31+1.3)^2*(F31+G31+H31+0.15)*风机基础条件输入!$G$2/10</f>
+        <v>1227.5584798342904</v>
+      </c>
+      <c r="Q31" s="49">
+        <f>PI()*(C31+1.3)^2*(F31+G31+H31+0.15)*风机基础条件输入!$H$2/10</f>
+        <v>0</v>
+      </c>
+      <c r="R31" s="49">
         <f t="shared" si="0"/>
-        <v>283.5287369864788</v>
-      </c>
-      <c r="P31" s="23">
-        <f t="shared" si="1"/>
-        <v>391.49421944391548</v>
-      </c>
-      <c r="Q31" s="23">
-        <f t="shared" si="2"/>
-        <v>43.429376843225299</v>
-      </c>
-      <c r="R31" s="23">
-        <f>PI()*(E31+1.3)^2*(H31+I31+J31+0.15)*风机基础条件输入!$G$2/10</f>
-        <v>1227.5584798342904</v>
-      </c>
-      <c r="S31" s="23">
-        <f>PI()*(E31+1.3)^2*(H31+I31+J31+0.15)*风机基础条件输入!$H$2/10</f>
-        <v>0</v>
-      </c>
-      <c r="T31" s="23">
-        <f t="shared" si="3"/>
         <v>792.63488354714968</v>
       </c>
-      <c r="U31" s="23"/>
-    </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.15">
-      <c r="A32">
+      <c r="S31" s="23"/>
+      <c r="U31">
         <v>7</v>
       </c>
-      <c r="B32">
+      <c r="V31">
         <v>120</v>
       </c>
-      <c r="C32" s="24" t="s">
+    </row>
+    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A32" s="45" t="s">
         <v>37</v>
       </c>
-      <c r="D32" s="20">
+      <c r="B32" s="45">
         <v>80000</v>
       </c>
+      <c r="C32" s="2">
+        <v>10</v>
+      </c>
+      <c r="D32" s="2">
+        <v>4</v>
+      </c>
       <c r="E32" s="2">
+        <v>4</v>
+      </c>
+      <c r="F32" s="2">
+        <v>1</v>
+      </c>
+      <c r="G32" s="22">
+        <v>1.4</v>
+      </c>
+      <c r="H32" s="22">
+        <v>1</v>
+      </c>
+      <c r="I32" s="22">
+        <v>0.6</v>
+      </c>
+      <c r="J32" s="22">
+        <v>26</v>
+      </c>
+      <c r="K32" s="22">
         <v>10</v>
       </c>
-      <c r="F32" s="2">
-        <v>4</v>
-      </c>
-      <c r="G32" s="2">
-        <v>4</v>
-      </c>
-      <c r="H32" s="2">
-        <v>1</v>
-      </c>
-      <c r="I32" s="22">
-        <v>1.4</v>
-      </c>
-      <c r="J32" s="22">
-        <v>1</v>
-      </c>
-      <c r="K32" s="22">
-        <v>0.6</v>
-      </c>
       <c r="L32" s="22">
-        <v>26</v>
-      </c>
-      <c r="M32" s="22">
-        <v>10</v>
-      </c>
-      <c r="N32" s="22">
         <f t="shared" si="4"/>
         <v>260</v>
       </c>
-      <c r="O32" s="23">
+      <c r="M32" s="49">
+        <f t="shared" si="1"/>
+        <v>314.15926535897933</v>
+      </c>
+      <c r="N32" s="49">
+        <f t="shared" si="2"/>
+        <v>437.22474781641603</v>
+      </c>
+      <c r="O32" s="49">
+        <f t="shared" si="3"/>
+        <v>48.071079988904216</v>
+      </c>
+      <c r="P32" s="49">
+        <f>PI()*(C32+1.3)^2*(F32+G32+H32+0.15)*风机基础条件输入!$G$2/10</f>
+        <v>1424.0823790759266</v>
+      </c>
+      <c r="Q32" s="49">
+        <f>PI()*(C32+1.3)^2*(F32+G32+H32+0.15)*风机基础条件输入!$H$2/10</f>
+        <v>0</v>
+      </c>
+      <c r="R32" s="49">
         <f t="shared" si="0"/>
-        <v>314.15926535897933</v>
-      </c>
-      <c r="P32" s="23">
-        <f t="shared" si="1"/>
-        <v>437.22474781641603</v>
-      </c>
-      <c r="Q32" s="23">
-        <f t="shared" si="2"/>
-        <v>48.071079988904216</v>
-      </c>
-      <c r="R32" s="23">
-        <f>PI()*(E32+1.3)^2*(H32+I32+J32+0.15)*风机基础条件输入!$G$2/10</f>
-        <v>1424.0823790759266</v>
-      </c>
-      <c r="S32" s="23">
-        <f>PI()*(E32+1.3)^2*(H32+I32+J32+0.15)*风机基础条件输入!$H$2/10</f>
-        <v>0</v>
-      </c>
-      <c r="T32" s="23">
-        <f t="shared" si="3"/>
         <v>938.78655127060631</v>
       </c>
-      <c r="U32" s="23"/>
-    </row>
-    <row r="33" spans="1:21" x14ac:dyDescent="0.15">
-      <c r="A33">
+      <c r="S32" s="23"/>
+      <c r="U32">
         <v>7</v>
       </c>
-      <c r="B33">
+      <c r="V32">
         <v>120</v>
       </c>
-      <c r="C33" s="24" t="s">
+    </row>
+    <row r="33" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A33" s="45" t="s">
         <v>37</v>
       </c>
-      <c r="D33" s="20">
+      <c r="B33" s="45">
         <v>90000</v>
       </c>
+      <c r="C33" s="2">
+        <v>10</v>
+      </c>
+      <c r="D33" s="2">
+        <v>4</v>
+      </c>
       <c r="E33" s="2">
+        <v>4</v>
+      </c>
+      <c r="F33" s="2">
+        <v>1</v>
+      </c>
+      <c r="G33" s="22">
+        <v>1.4</v>
+      </c>
+      <c r="H33" s="22">
+        <v>1</v>
+      </c>
+      <c r="I33" s="22">
+        <v>0.6</v>
+      </c>
+      <c r="J33" s="22">
+        <v>28</v>
+      </c>
+      <c r="K33" s="22">
         <v>10</v>
       </c>
-      <c r="F33" s="2">
-        <v>4</v>
-      </c>
-      <c r="G33" s="2">
-        <v>4</v>
-      </c>
-      <c r="H33" s="2">
-        <v>1</v>
-      </c>
-      <c r="I33" s="22">
-        <v>1.4</v>
-      </c>
-      <c r="J33" s="22">
-        <v>1</v>
-      </c>
-      <c r="K33" s="22">
-        <v>0.6</v>
-      </c>
       <c r="L33" s="22">
-        <v>28</v>
-      </c>
-      <c r="M33" s="22">
-        <v>10</v>
-      </c>
-      <c r="N33" s="22">
         <f t="shared" si="4"/>
         <v>280</v>
       </c>
-      <c r="O33" s="23">
+      <c r="M33" s="49">
+        <f t="shared" si="1"/>
+        <v>314.15926535897933</v>
+      </c>
+      <c r="N33" s="49">
+        <f t="shared" si="2"/>
+        <v>437.22474781641603</v>
+      </c>
+      <c r="O33" s="49">
+        <f t="shared" si="3"/>
+        <v>48.071079988904216</v>
+      </c>
+      <c r="P33" s="49">
+        <f>PI()*(C33+1.3)^2*(F33+G33+H33+0.15)*风机基础条件输入!$G$2/10</f>
+        <v>1424.0823790759266</v>
+      </c>
+      <c r="Q33" s="49">
+        <f>PI()*(C33+1.3)^2*(F33+G33+H33+0.15)*风机基础条件输入!$H$2/10</f>
+        <v>0</v>
+      </c>
+      <c r="R33" s="49">
         <f t="shared" si="0"/>
-        <v>314.15926535897933</v>
-      </c>
-      <c r="P33" s="23">
-        <f t="shared" si="1"/>
-        <v>437.22474781641603</v>
-      </c>
-      <c r="Q33" s="23">
-        <f t="shared" si="2"/>
-        <v>48.071079988904216</v>
-      </c>
-      <c r="R33" s="23">
-        <f>PI()*(E33+1.3)^2*(H33+I33+J33+0.15)*风机基础条件输入!$G$2/10</f>
-        <v>1424.0823790759266</v>
-      </c>
-      <c r="S33" s="23">
-        <f>PI()*(E33+1.3)^2*(H33+I33+J33+0.15)*风机基础条件输入!$H$2/10</f>
-        <v>0</v>
-      </c>
-      <c r="T33" s="23">
-        <f t="shared" si="3"/>
         <v>938.78655127060631</v>
       </c>
-      <c r="U33" s="23"/>
-    </row>
-    <row r="34" spans="1:21" x14ac:dyDescent="0.15">
-      <c r="A34">
+      <c r="S33" s="23"/>
+      <c r="U33">
         <v>7</v>
       </c>
-      <c r="B34">
+      <c r="V33">
         <v>120</v>
       </c>
-      <c r="C34" s="24" t="s">
+    </row>
+    <row r="34" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A34" s="45" t="s">
         <v>37</v>
       </c>
-      <c r="D34" s="20">
+      <c r="B34" s="45">
         <v>100000</v>
       </c>
-      <c r="E34" s="1">
+      <c r="C34" s="1">
         <v>10.25</v>
       </c>
+      <c r="D34" s="2">
+        <v>4</v>
+      </c>
+      <c r="E34" s="2">
+        <v>4</v>
+      </c>
       <c r="F34" s="2">
-        <v>4</v>
-      </c>
-      <c r="G34" s="2">
-        <v>4</v>
-      </c>
-      <c r="H34" s="2">
         <v>1.1000000000000001</v>
       </c>
+      <c r="G34" s="22">
+        <v>1.4</v>
+      </c>
+      <c r="H34" s="22">
+        <v>1</v>
+      </c>
       <c r="I34" s="22">
-        <v>1.4</v>
+        <v>0.6</v>
       </c>
       <c r="J34" s="22">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="K34" s="22">
-        <v>0.6</v>
+        <v>10</v>
       </c>
       <c r="L34" s="22">
-        <v>30</v>
-      </c>
-      <c r="M34" s="22">
-        <v>10</v>
-      </c>
-      <c r="N34" s="22">
         <f t="shared" si="4"/>
         <v>300</v>
       </c>
-      <c r="O34" s="23">
+      <c r="M34" s="49">
+        <f t="shared" si="1"/>
+        <v>330.06357816777762</v>
+      </c>
+      <c r="N34" s="49">
+        <f t="shared" si="2"/>
+        <v>488.96458510865875</v>
+      </c>
+      <c r="O34" s="49">
+        <f t="shared" si="3"/>
+        <v>50.480288855125885</v>
+      </c>
+      <c r="P34" s="49">
+        <f>PI()*(C34+1.3)^2*(F34+G34+H34+0.15)*风机基础条件输入!$G$2/10</f>
+        <v>1529.70154599237</v>
+      </c>
+      <c r="Q34" s="49">
+        <f>PI()*(C34+1.3)^2*(F34+G34+H34+0.15)*风机基础条件输入!$H$2/10</f>
+        <v>0</v>
+      </c>
+      <c r="R34" s="49">
         <f t="shared" si="0"/>
-        <v>330.06357816777762</v>
-      </c>
-      <c r="P34" s="23">
-        <f t="shared" si="1"/>
-        <v>488.96458510865875</v>
-      </c>
-      <c r="Q34" s="23">
-        <f t="shared" si="2"/>
-        <v>50.480288855125885</v>
-      </c>
-      <c r="R34" s="23">
-        <f>PI()*(E34+1.3)^2*(H34+I34+J34+0.15)*风机基础条件输入!$G$2/10</f>
-        <v>1529.70154599237</v>
-      </c>
-      <c r="S34" s="23">
-        <f>PI()*(E34+1.3)^2*(H34+I34+J34+0.15)*风机基础条件输入!$H$2/10</f>
-        <v>0</v>
-      </c>
-      <c r="T34" s="23">
-        <f t="shared" si="3"/>
         <v>990.25667202858529</v>
       </c>
-      <c r="U34" s="23"/>
-    </row>
-    <row r="35" spans="1:21" x14ac:dyDescent="0.15">
-      <c r="A35">
+      <c r="S34" s="23"/>
+      <c r="U34">
         <v>7</v>
       </c>
-      <c r="B35">
+      <c r="V34">
         <v>120</v>
       </c>
-      <c r="C35" s="24" t="s">
+    </row>
+    <row r="35" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A35" s="45" t="s">
         <v>37</v>
       </c>
-      <c r="D35" s="20">
+      <c r="B35" s="45">
         <v>110000</v>
       </c>
-      <c r="E35" s="1">
+      <c r="C35" s="1">
         <v>10.25</v>
       </c>
+      <c r="D35" s="2">
+        <v>4</v>
+      </c>
+      <c r="E35" s="2">
+        <v>4</v>
+      </c>
       <c r="F35" s="2">
-        <v>4</v>
-      </c>
-      <c r="G35" s="2">
-        <v>4</v>
-      </c>
-      <c r="H35" s="2">
         <v>1.1000000000000001</v>
       </c>
+      <c r="G35" s="22">
+        <v>1.4</v>
+      </c>
+      <c r="H35" s="22">
+        <v>1</v>
+      </c>
       <c r="I35" s="22">
-        <v>1.4</v>
+        <v>0.6</v>
       </c>
       <c r="J35" s="22">
-        <v>1</v>
+        <v>32</v>
       </c>
       <c r="K35" s="22">
-        <v>0.6</v>
+        <v>10</v>
       </c>
       <c r="L35" s="22">
-        <v>32</v>
-      </c>
-      <c r="M35" s="22">
-        <v>10</v>
-      </c>
-      <c r="N35" s="22">
         <f t="shared" si="4"/>
         <v>320</v>
       </c>
-      <c r="O35" s="23">
+      <c r="M35" s="49">
+        <f t="shared" si="1"/>
+        <v>330.06357816777762</v>
+      </c>
+      <c r="N35" s="49">
+        <f t="shared" si="2"/>
+        <v>488.96458510865875</v>
+      </c>
+      <c r="O35" s="49">
+        <f t="shared" si="3"/>
+        <v>50.480288855125885</v>
+      </c>
+      <c r="P35" s="49">
+        <f>PI()*(C35+1.3)^2*(F35+G35+H35+0.15)*风机基础条件输入!$G$2/10</f>
+        <v>1529.70154599237</v>
+      </c>
+      <c r="Q35" s="49">
+        <f>PI()*(C35+1.3)^2*(F35+G35+H35+0.15)*风机基础条件输入!$H$2/10</f>
+        <v>0</v>
+      </c>
+      <c r="R35" s="49">
         <f t="shared" si="0"/>
-        <v>330.06357816777762</v>
-      </c>
-      <c r="P35" s="23">
-        <f t="shared" si="1"/>
-        <v>488.96458510865875</v>
-      </c>
-      <c r="Q35" s="23">
-        <f t="shared" si="2"/>
-        <v>50.480288855125885</v>
-      </c>
-      <c r="R35" s="23">
-        <f>PI()*(E35+1.3)^2*(H35+I35+J35+0.15)*风机基础条件输入!$G$2/10</f>
-        <v>1529.70154599237</v>
-      </c>
-      <c r="S35" s="23">
-        <f>PI()*(E35+1.3)^2*(H35+I35+J35+0.15)*风机基础条件输入!$H$2/10</f>
-        <v>0</v>
-      </c>
-      <c r="T35" s="23">
-        <f t="shared" si="3"/>
         <v>990.25667202858529</v>
       </c>
-      <c r="U35" s="23"/>
-    </row>
-    <row r="36" spans="1:21" x14ac:dyDescent="0.15">
-      <c r="A36">
+      <c r="S35" s="23"/>
+      <c r="U35">
         <v>7</v>
       </c>
-      <c r="B36">
+      <c r="V35">
         <v>120</v>
       </c>
-      <c r="C36" s="24" t="s">
+    </row>
+    <row r="36" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A36" s="45" t="s">
         <v>37</v>
       </c>
-      <c r="D36" s="20">
+      <c r="B36" s="45">
         <v>120000</v>
       </c>
-      <c r="E36" s="21">
+      <c r="C36" s="21">
         <v>10.5</v>
       </c>
+      <c r="D36" s="2">
+        <v>4</v>
+      </c>
+      <c r="E36" s="2">
+        <v>4</v>
+      </c>
       <c r="F36" s="2">
-        <v>4</v>
-      </c>
-      <c r="G36" s="2">
-        <v>4</v>
-      </c>
-      <c r="H36" s="2">
         <v>1.2</v>
       </c>
+      <c r="G36" s="22">
+        <v>1.4</v>
+      </c>
+      <c r="H36" s="22">
+        <v>1</v>
+      </c>
       <c r="I36" s="22">
-        <v>1.4</v>
+        <v>0.6</v>
       </c>
       <c r="J36" s="22">
-        <v>1</v>
+        <v>34</v>
       </c>
       <c r="K36" s="22">
-        <v>0.6</v>
+        <v>10</v>
       </c>
       <c r="L36" s="22">
-        <v>34</v>
-      </c>
-      <c r="M36" s="22">
-        <v>10</v>
-      </c>
-      <c r="N36" s="22">
         <f t="shared" si="4"/>
         <v>340</v>
       </c>
-      <c r="O36" s="23">
+      <c r="M36" s="49">
+        <f t="shared" si="1"/>
+        <v>346.36059005827468</v>
+      </c>
+      <c r="N36" s="49">
+        <f t="shared" si="2"/>
+        <v>544.41485719403295</v>
+      </c>
+      <c r="O36" s="49">
+        <f t="shared" si="3"/>
+        <v>52.948402583602373</v>
+      </c>
+      <c r="P36" s="49">
+        <f>PI()*(C36+1.3)^2*(F36+G36+H36+0.15)*风机基础条件输入!$G$2/10</f>
+        <v>1640.3826040719105</v>
+      </c>
+      <c r="Q36" s="49">
+        <f>PI()*(C36+1.3)^2*(F36+G36+H36+0.15)*风机基础条件输入!$H$2/10</f>
+        <v>0</v>
+      </c>
+      <c r="R36" s="49">
         <f t="shared" si="0"/>
-        <v>346.36059005827468</v>
-      </c>
-      <c r="P36" s="23">
-        <f t="shared" si="1"/>
-        <v>544.41485719403295</v>
-      </c>
-      <c r="Q36" s="23">
-        <f t="shared" si="2"/>
-        <v>52.948402583602373</v>
-      </c>
-      <c r="R36" s="23">
-        <f>PI()*(E36+1.3)^2*(H36+I36+J36+0.15)*风机基础条件输入!$G$2/10</f>
-        <v>1640.3826040719105</v>
-      </c>
-      <c r="S36" s="23">
-        <f>PI()*(E36+1.3)^2*(H36+I36+J36+0.15)*风机基础条件输入!$H$2/10</f>
-        <v>0</v>
-      </c>
-      <c r="T36" s="23">
-        <f t="shared" si="3"/>
         <v>1043.0193442942752</v>
       </c>
-      <c r="U36" s="23"/>
+      <c r="S36" s="23"/>
+      <c r="U36">
+        <v>7</v>
+      </c>
+      <c r="V36">
+        <v>120</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
</xml_diff>